<commit_message>
added ejs, started to add templating
</commit_message>
<xml_diff>
--- a/public/Modultafel_Template.xlsx
+++ b/public/Modultafel_Template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Laurent\IdeaProjects\Modultafel\public\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andrin.kappeler\Downloads\Modultafel\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7754D266-A68D-47FB-90D0-E3351A54D501}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39ED1A96-ECEA-4238-88E4-4058F4C38F4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="51976" yWindow="0" windowWidth="17579" windowHeight="18937" activeTab="1" xr2:uid="{C0A2E809-DD1F-47D3-9648-758D3A48BE07}"/>
+    <workbookView xWindow="4560" yWindow="4560" windowWidth="10150" windowHeight="6560" xr2:uid="{C0A2E809-DD1F-47D3-9648-758D3A48BE07}"/>
   </bookViews>
   <sheets>
     <sheet name="Einstellungen" sheetId="2" r:id="rId1"/>
@@ -736,19 +736,19 @@
   </sheetPr>
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="18.125" customWidth="1"/>
+    <col min="1" max="1" width="18.08984375" customWidth="1"/>
     <col min="3" max="3" width="14" customWidth="1"/>
-    <col min="4" max="4" width="17.25" customWidth="1"/>
-    <col min="5" max="5" width="20.25" customWidth="1"/>
+    <col min="4" max="4" width="17.26953125" customWidth="1"/>
+    <col min="5" max="5" width="20.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -762,7 +762,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -776,7 +776,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -790,7 +790,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -804,7 +804,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -818,22 +818,22 @@
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -852,23 +852,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F05469D6-429B-4FE2-AB98-8A05D5510F8C}">
   <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12.625" customWidth="1"/>
+    <col min="1" max="1" width="12.6328125" customWidth="1"/>
     <col min="2" max="2" width="14" customWidth="1"/>
-    <col min="3" max="3" width="22.875" customWidth="1"/>
-    <col min="4" max="4" width="46.75" customWidth="1"/>
-    <col min="5" max="5" width="18.25" customWidth="1"/>
-    <col min="6" max="6" width="9.25" customWidth="1"/>
-    <col min="7" max="7" width="97.25" customWidth="1"/>
-    <col min="9" max="9" width="93.75" customWidth="1"/>
+    <col min="3" max="3" width="22.90625" customWidth="1"/>
+    <col min="4" max="4" width="46.7265625" customWidth="1"/>
+    <col min="5" max="5" width="18.26953125" customWidth="1"/>
+    <col min="6" max="6" width="9.26953125" customWidth="1"/>
+    <col min="7" max="7" width="97.26953125" customWidth="1"/>
+    <col min="9" max="9" width="93.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -891,7 +891,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -911,7 +911,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -931,7 +931,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -951,7 +951,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -971,7 +971,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -991,7 +991,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -1011,7 +1011,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -1031,7 +1031,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -1051,7 +1051,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -1071,7 +1071,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -1091,7 +1091,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>9</v>
       </c>
@@ -1111,7 +1111,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>9</v>
       </c>
@@ -1179,15 +1179,15 @@
       <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="19" customWidth="1"/>
-    <col min="2" max="2" width="19.5" customWidth="1"/>
-    <col min="3" max="3" width="28.25" customWidth="1"/>
-    <col min="4" max="4" width="28.375" customWidth="1"/>
+    <col min="2" max="2" width="19.453125" customWidth="1"/>
+    <col min="3" max="3" width="28.26953125" customWidth="1"/>
+    <col min="4" max="4" width="28.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
Updated style of genereated Modultafel. Printing with color now working by removing @Media print tags in style.ejs. Added new Text fields to Excel template
</commit_message>
<xml_diff>
--- a/public/Modultafel_Template.xlsx
+++ b/public/Modultafel_Template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andri\IdeaProjects\Modultafel\public\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Laurent\IdeaProjects\Modultafel\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFAB25B7-D7F7-41C3-9B2C-146AFB2C963F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64DFD2D4-D0EC-4607-AAA2-05ED481B060F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{C0A2E809-DD1F-47D3-9648-758D3A48BE07}"/>
+    <workbookView xWindow="40306" yWindow="0" windowWidth="17579" windowHeight="18842" xr2:uid="{C0A2E809-DD1F-47D3-9648-758D3A48BE07}"/>
   </bookViews>
   <sheets>
     <sheet name="Einstellungen" sheetId="2" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="78">
   <si>
     <t>ECTS</t>
   </si>
@@ -238,6 +238,38 @@
   </si>
   <si>
     <t>#EB6E0C</t>
+  </si>
+  <si>
+    <t>InfoTextOben</t>
+  </si>
+  <si>
+    <t>WarningTextOben</t>
+  </si>
+  <si>
+    <t>InfoTextUnten</t>
+  </si>
+  <si>
+    <t>WarningTextWPM</t>
+  </si>
+  <si>
+    <t>Dies ist ein Informations-text Beispiel</t>
+  </si>
+  <si>
+    <t>Dies ist ein Warnungs-text Beispiel</t>
+  </si>
+  <si>
+    <t>* = Dieses Modul wird in englischer Sprache durchgeführt
+Drucktipps: Stellen Sie in der Druckansicht sicher, dass die Option "Querformat" aktiviert ist und die Seitenränder in den Seiteneigenschaften auf 0 gesetzt sind.</t>
+  </si>
+  <si>
+    <t>Die Modulbeschreibungen sind aktuell in Überarbeitung und stehen Ihnen ab Montag, 21. November 2022 zur Verfügung.</t>
+  </si>
+  <si>
+    <t>Modultafel Bachelorstudiengang Wirtschaftsinformatik
+Vollzeit, ab Herbstsemester 2014</t>
+  </si>
+  <si>
+    <t>Titel</t>
   </si>
 </sst>
 </file>
@@ -279,13 +311,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="9">
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -419,16 +457,30 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{CF4ACF50-5041-4410-9F27-503054A8E586}" name="Tabelle1" displayName="Tabelle1" ref="A1:G1048575" totalsRowShown="0" dataDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{3A4F6131-954A-4F6B-BC51-8E9A8FDF27E9}" name="Tabelle4" displayName="Tabelle4" ref="G1:K2" totalsRowShown="0">
+  <autoFilter ref="G1:K2" xr:uid="{3A4F6131-954A-4F6B-BC51-8E9A8FDF27E9}"/>
+  <tableColumns count="5">
+    <tableColumn id="5" xr3:uid="{24A2282B-9BBC-42A7-A34E-0FD0F404A30A}" name="Titel" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{535AB875-9018-45C5-9F43-A4487869B22E}" name="InfoTextOben"/>
+    <tableColumn id="2" xr3:uid="{2384252E-6755-42FC-BE4B-94373EF66A69}" name="WarningTextOben"/>
+    <tableColumn id="3" xr3:uid="{F4FF534A-8B3C-4A06-AF0D-46BA4D277D9C}" name="InfoTextUnten"/>
+    <tableColumn id="4" xr3:uid="{48B9B103-D91B-4639-BD23-E0858AFC5F5D}" name="WarningTextWPM"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{CF4ACF50-5041-4410-9F27-503054A8E586}" name="Tabelle1" displayName="Tabelle1" ref="A1:G1048575" totalsRowShown="0" dataDxfId="8">
   <autoFilter ref="A1:G1048575" xr:uid="{CF4ACF50-5041-4410-9F27-503054A8E586}"/>
   <tableColumns count="7">
-    <tableColumn id="6" xr3:uid="{E6C1C015-3DB3-47F6-929A-743509FD5797}" name="Semester" dataDxfId="6"/>
-    <tableColumn id="5" xr3:uid="{5E3B9891-0394-4C86-AC02-0F20186B6BAF}" name="Modulgruppe" dataDxfId="5"/>
-    <tableColumn id="1" xr3:uid="{50DDDC12-2C42-44A4-850B-86543C944BDA}" name="Modulkuerzel" dataDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{07E784E3-5360-4D49-8705-EE742D1C517A}" name="Modulbezeichnung" dataDxfId="3"/>
-    <tableColumn id="9" xr3:uid="{4328C022-5756-4282-B959-03E01B81440F}" name="Wahlpflichtmodul" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{8D13C487-08ED-4D82-91C4-0A680804285D}" name="ECTS" dataDxfId="1"/>
-    <tableColumn id="4" xr3:uid="{14712FC0-3A9A-4960-AC0D-0685592D6EEC}" name="Link" dataDxfId="0">
+    <tableColumn id="6" xr3:uid="{E6C1C015-3DB3-47F6-929A-743509FD5797}" name="Semester" dataDxfId="7"/>
+    <tableColumn id="5" xr3:uid="{5E3B9891-0394-4C86-AC02-0F20186B6BAF}" name="Modulgruppe" dataDxfId="6"/>
+    <tableColumn id="1" xr3:uid="{50DDDC12-2C42-44A4-850B-86543C944BDA}" name="Modulkuerzel" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{07E784E3-5360-4D49-8705-EE742D1C517A}" name="Modulbezeichnung" dataDxfId="4"/>
+    <tableColumn id="9" xr3:uid="{4328C022-5756-4282-B959-03E01B81440F}" name="Wahlpflichtmodul" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{8D13C487-08ED-4D82-91C4-0A680804285D}" name="ECTS" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{14712FC0-3A9A-4960-AC0D-0685592D6EEC}" name="Link" dataDxfId="1">
       <calculatedColumnFormula>IF(Tabelle1[[#This Row],[Modulkuerzel]] &lt;&gt; "",HYPERLINK(CONCATENATE("https://modulmanagement.sml.zhaw.ch/StaticModDescAblage/Modulbeschreibung_",Tabelle1[[#This Row],[Modulkuerzel]],".pdf")), null)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -437,7 +489,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -736,21 +788,25 @@
   <sheetPr>
     <tabColor theme="1" tint="0.14999847407452621"/>
   </sheetPr>
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:K9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.08984375" customWidth="1"/>
+    <col min="1" max="1" width="18.125" customWidth="1"/>
     <col min="3" max="3" width="14" customWidth="1"/>
-    <col min="4" max="4" width="17.26953125" customWidth="1"/>
-    <col min="5" max="5" width="20.26953125" customWidth="1"/>
+    <col min="4" max="4" width="17.25" customWidth="1"/>
+    <col min="5" max="6" width="20.25" customWidth="1"/>
+    <col min="7" max="8" width="33.125" customWidth="1"/>
+    <col min="10" max="10" width="33.125" customWidth="1"/>
+    <col min="11" max="11" width="102.875" customWidth="1"/>
+    <col min="12" max="12" width="33.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -763,8 +819,23 @@
       <c r="E1" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="G1" t="s">
+        <v>77</v>
+      </c>
+      <c r="H1" t="s">
+        <v>68</v>
+      </c>
+      <c r="I1" t="s">
+        <v>69</v>
+      </c>
+      <c r="J1" t="s">
+        <v>70</v>
+      </c>
+      <c r="K1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="18.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -777,8 +848,23 @@
       <c r="E2" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="G2" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="H2" t="s">
+        <v>72</v>
+      </c>
+      <c r="I2" t="s">
+        <v>73</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="K2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="18.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -792,7 +878,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -806,7 +892,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -820,22 +906,22 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -843,9 +929,10 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <tableParts count="2">
+  <tableParts count="3">
     <tablePart r:id="rId1"/>
     <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
@@ -858,19 +945,19 @@
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.6328125" customWidth="1"/>
+    <col min="1" max="1" width="12.625" customWidth="1"/>
     <col min="2" max="2" width="14" customWidth="1"/>
-    <col min="3" max="3" width="22.90625" customWidth="1"/>
-    <col min="4" max="4" width="46.7265625" customWidth="1"/>
-    <col min="5" max="5" width="18.26953125" customWidth="1"/>
-    <col min="6" max="6" width="9.26953125" customWidth="1"/>
-    <col min="7" max="7" width="97.26953125" customWidth="1"/>
-    <col min="9" max="9" width="93.7265625" customWidth="1"/>
+    <col min="3" max="3" width="22.875" customWidth="1"/>
+    <col min="4" max="4" width="46.75" customWidth="1"/>
+    <col min="5" max="5" width="18.25" customWidth="1"/>
+    <col min="6" max="6" width="9.25" customWidth="1"/>
+    <col min="7" max="7" width="97.25" customWidth="1"/>
+    <col min="9" max="9" width="93.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -893,7 +980,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -913,7 +1000,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -933,7 +1020,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -953,7 +1040,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -973,7 +1060,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -993,7 +1080,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -1013,7 +1100,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -1033,7 +1120,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -1053,7 +1140,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -1073,7 +1160,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -1093,7 +1180,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>9</v>
       </c>
@@ -1113,7 +1200,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>9</v>
       </c>
@@ -1181,15 +1268,15 @@
       <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19" customWidth="1"/>
-    <col min="2" max="2" width="19.453125" customWidth="1"/>
-    <col min="3" max="3" width="28.26953125" customWidth="1"/>
-    <col min="4" max="4" width="28.36328125" customWidth="1"/>
+    <col min="2" max="2" width="19.5" customWidth="1"/>
+    <col min="3" max="3" width="28.25" customWidth="1"/>
+    <col min="4" max="4" width="28.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
Added font family and size to excel template file
</commit_message>
<xml_diff>
--- a/public/Modultafel_Template.xlsx
+++ b/public/Modultafel_Template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Laurent\IdeaProjects\Modultafel\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64DFD2D4-D0EC-4607-AAA2-05ED481B060F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8F25E9B-63C7-4383-A19C-03B6377199C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="40306" yWindow="0" windowWidth="17579" windowHeight="18842" xr2:uid="{C0A2E809-DD1F-47D3-9648-758D3A48BE07}"/>
+    <workbookView xWindow="40469" yWindow="421" windowWidth="17579" windowHeight="18842" xr2:uid="{C0A2E809-DD1F-47D3-9648-758D3A48BE07}"/>
   </bookViews>
   <sheets>
     <sheet name="Einstellungen" sheetId="2" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="82">
   <si>
     <t>ECTS</t>
   </si>
@@ -270,6 +270,18 @@
   </si>
   <si>
     <t>Titel</t>
+  </si>
+  <si>
+    <t>FontSize</t>
+  </si>
+  <si>
+    <t>FontFamily</t>
+  </si>
+  <si>
+    <t>Arial, Helvetica, sans-serif</t>
+  </si>
+  <si>
+    <t>0.6rem</t>
   </si>
 </sst>
 </file>
@@ -321,9 +333,6 @@
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="9">
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -421,6 +430,9 @@
         <scheme val="minor"/>
       </font>
     </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -460,7 +472,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{3A4F6131-954A-4F6B-BC51-8E9A8FDF27E9}" name="Tabelle4" displayName="Tabelle4" ref="G1:K2" totalsRowShown="0">
   <autoFilter ref="G1:K2" xr:uid="{3A4F6131-954A-4F6B-BC51-8E9A8FDF27E9}"/>
   <tableColumns count="5">
-    <tableColumn id="5" xr3:uid="{24A2282B-9BBC-42A7-A34E-0FD0F404A30A}" name="Titel" dataDxfId="0"/>
+    <tableColumn id="5" xr3:uid="{24A2282B-9BBC-42A7-A34E-0FD0F404A30A}" name="Titel" dataDxfId="8"/>
     <tableColumn id="1" xr3:uid="{535AB875-9018-45C5-9F43-A4487869B22E}" name="InfoTextOben"/>
     <tableColumn id="2" xr3:uid="{2384252E-6755-42FC-BE4B-94373EF66A69}" name="WarningTextOben"/>
     <tableColumn id="3" xr3:uid="{F4FF534A-8B3C-4A06-AF0D-46BA4D277D9C}" name="InfoTextUnten"/>
@@ -471,16 +483,27 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{CF4ACF50-5041-4410-9F27-503054A8E586}" name="Tabelle1" displayName="Tabelle1" ref="A1:G1048575" totalsRowShown="0" dataDxfId="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{29B5C5B2-6743-42FC-8083-8915EF4B9139}" name="Tabelle5" displayName="Tabelle5" ref="M1:N2" totalsRowShown="0">
+  <autoFilter ref="M1:N2" xr:uid="{29B5C5B2-6743-42FC-8083-8915EF4B9139}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{BC4D296C-6336-436B-B850-FD3B6BC395F2}" name="FontFamily"/>
+    <tableColumn id="2" xr3:uid="{5BA600E0-17A6-4994-B4BF-339A9FE90433}" name="FontSize"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight12" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{CF4ACF50-5041-4410-9F27-503054A8E586}" name="Tabelle1" displayName="Tabelle1" ref="A1:G1048575" totalsRowShown="0" dataDxfId="7">
   <autoFilter ref="A1:G1048575" xr:uid="{CF4ACF50-5041-4410-9F27-503054A8E586}"/>
   <tableColumns count="7">
-    <tableColumn id="6" xr3:uid="{E6C1C015-3DB3-47F6-929A-743509FD5797}" name="Semester" dataDxfId="7"/>
-    <tableColumn id="5" xr3:uid="{5E3B9891-0394-4C86-AC02-0F20186B6BAF}" name="Modulgruppe" dataDxfId="6"/>
-    <tableColumn id="1" xr3:uid="{50DDDC12-2C42-44A4-850B-86543C944BDA}" name="Modulkuerzel" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{07E784E3-5360-4D49-8705-EE742D1C517A}" name="Modulbezeichnung" dataDxfId="4"/>
-    <tableColumn id="9" xr3:uid="{4328C022-5756-4282-B959-03E01B81440F}" name="Wahlpflichtmodul" dataDxfId="3"/>
-    <tableColumn id="3" xr3:uid="{8D13C487-08ED-4D82-91C4-0A680804285D}" name="ECTS" dataDxfId="2"/>
-    <tableColumn id="4" xr3:uid="{14712FC0-3A9A-4960-AC0D-0685592D6EEC}" name="Link" dataDxfId="1">
+    <tableColumn id="6" xr3:uid="{E6C1C015-3DB3-47F6-929A-743509FD5797}" name="Semester" dataDxfId="6"/>
+    <tableColumn id="5" xr3:uid="{5E3B9891-0394-4C86-AC02-0F20186B6BAF}" name="Modulgruppe" dataDxfId="5"/>
+    <tableColumn id="1" xr3:uid="{50DDDC12-2C42-44A4-850B-86543C944BDA}" name="Modulkuerzel" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{07E784E3-5360-4D49-8705-EE742D1C517A}" name="Modulbezeichnung" dataDxfId="3"/>
+    <tableColumn id="9" xr3:uid="{4328C022-5756-4282-B959-03E01B81440F}" name="Wahlpflichtmodul" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{8D13C487-08ED-4D82-91C4-0A680804285D}" name="ECTS" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{14712FC0-3A9A-4960-AC0D-0685592D6EEC}" name="Link" dataDxfId="0">
       <calculatedColumnFormula>IF(Tabelle1[[#This Row],[Modulkuerzel]] &lt;&gt; "",HYPERLINK(CONCATENATE("https://modulmanagement.sml.zhaw.ch/StaticModDescAblage/Modulbeschreibung_",Tabelle1[[#This Row],[Modulkuerzel]],".pdf")), null)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -788,10 +811,10 @@
   <sheetPr>
     <tabColor theme="1" tint="0.14999847407452621"/>
   </sheetPr>
-  <dimension ref="A1:K9"/>
+  <dimension ref="A1:N9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K20" sqref="K20"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -804,9 +827,10 @@
     <col min="10" max="10" width="33.125" customWidth="1"/>
     <col min="11" max="11" width="102.875" customWidth="1"/>
     <col min="12" max="12" width="33.125" customWidth="1"/>
+    <col min="13" max="13" width="24.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -834,8 +858,14 @@
       <c r="K1" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" ht="18.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M1" t="s">
+        <v>79</v>
+      </c>
+      <c r="N1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" ht="18.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -863,8 +893,14 @@
       <c r="K2" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" ht="18.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M2" t="s">
+        <v>80</v>
+      </c>
+      <c r="N2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" ht="18.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -878,7 +914,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -892,7 +928,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -906,22 +942,22 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -929,10 +965,11 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <tableParts count="3">
+  <tableParts count="4">
     <tablePart r:id="rId1"/>
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Update colors to ZHAW Farbpalette and added Font color
</commit_message>
<xml_diff>
--- a/public/Modultafel_Template.xlsx
+++ b/public/Modultafel_Template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Laurent\IdeaProjects\Modultafel\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8F25E9B-63C7-4383-A19C-03B6377199C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F901CE70-3219-45C7-BF90-7BAC60272341}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="40469" yWindow="421" windowWidth="17579" windowHeight="18842" xr2:uid="{C0A2E809-DD1F-47D3-9648-758D3A48BE07}"/>
+    <workbookView xWindow="20676" yWindow="0" windowWidth="17579" windowHeight="18842" activeTab="1" xr2:uid="{C0A2E809-DD1F-47D3-9648-758D3A48BE07}"/>
   </bookViews>
   <sheets>
     <sheet name="Einstellungen" sheetId="2" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="85">
   <si>
     <t>ECTS</t>
   </si>
@@ -87,18 +87,6 @@
     <t>Hintergrundfarbe</t>
   </si>
   <si>
-    <t>Blau</t>
-  </si>
-  <si>
-    <t>Gelb</t>
-  </si>
-  <si>
-    <t>Orange</t>
-  </si>
-  <si>
-    <t>#FFF7DB</t>
-  </si>
-  <si>
     <t>Wahlpflichtmodul</t>
   </si>
   <si>
@@ -111,27 +99,6 @@
     <t>w.BA.XX.2BWL-WIN.XX</t>
   </si>
   <si>
-    <t>Hellblau</t>
-  </si>
-  <si>
-    <t>#0065A6</t>
-  </si>
-  <si>
-    <t>#ECECED</t>
-  </si>
-  <si>
-    <t>#FDE4D0</t>
-  </si>
-  <si>
-    <t>#D0DBEC</t>
-  </si>
-  <si>
-    <t>#6799C7</t>
-  </si>
-  <si>
-    <t>#FFD304</t>
-  </si>
-  <si>
     <t>Einführung Wirtschaftsinformatik</t>
   </si>
   <si>
@@ -235,9 +202,6 @@
   </si>
   <si>
     <t>FarbeModulkaestchen</t>
-  </si>
-  <si>
-    <t>#EB6E0C</t>
   </si>
   <si>
     <t>InfoTextOben</t>
@@ -282,13 +246,58 @@
   </si>
   <si>
     <t>0.6rem</t>
+  </si>
+  <si>
+    <t>Schriftfarbe</t>
+  </si>
+  <si>
+    <t>#FFFFFF</t>
+  </si>
+  <si>
+    <t>San Juan</t>
+  </si>
+  <si>
+    <t>#334771</t>
+  </si>
+  <si>
+    <t>#8f95b3</t>
+  </si>
+  <si>
+    <t>#000000</t>
+  </si>
+  <si>
+    <t>#a3d7e0</t>
+  </si>
+  <si>
+    <t>Pacific Blue</t>
+  </si>
+  <si>
+    <t>#00aebe</t>
+  </si>
+  <si>
+    <t>#90cec5</t>
+  </si>
+  <si>
+    <t>#cde8e2</t>
+  </si>
+  <si>
+    <t>Half Baked</t>
+  </si>
+  <si>
+    <t>#1e7cb8</t>
+  </si>
+  <si>
+    <t>#9db9dd</t>
+  </si>
+  <si>
+    <t>Eastern Blue</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -302,6 +311,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -311,7 +326,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -319,15 +334,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -457,20 +483,21 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{1518CA27-608D-4F3D-BA58-0F5BDD7E0903}" name="Tabelle3" displayName="Tabelle3" ref="C1:E358" totalsRowShown="0">
-  <autoFilter ref="C1:E358" xr:uid="{1518CA27-608D-4F3D-BA58-0F5BDD7E0903}"/>
-  <tableColumns count="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{1518CA27-608D-4F3D-BA58-0F5BDD7E0903}" name="Tabelle3" displayName="Tabelle3" ref="C1:F358" totalsRowShown="0">
+  <autoFilter ref="C1:F358" xr:uid="{1518CA27-608D-4F3D-BA58-0F5BDD7E0903}"/>
+  <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{30983517-1311-4A1A-86CE-52CFFBBD9602}" name="Modulgruppe"/>
     <tableColumn id="2" xr3:uid="{E38293F2-CBC1-4AB6-8F99-7A7998203608}" name="Hintergrundfarbe"/>
     <tableColumn id="3" xr3:uid="{9269A6E2-1D27-4CE5-89B5-81F0D1428B4F}" name="FarbeModulkaestchen"/>
+    <tableColumn id="4" xr3:uid="{54B9ECDC-10BF-483C-965A-107BDA4B655C}" name="Schriftfarbe"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{3A4F6131-954A-4F6B-BC51-8E9A8FDF27E9}" name="Tabelle4" displayName="Tabelle4" ref="G1:K2" totalsRowShown="0">
-  <autoFilter ref="G1:K2" xr:uid="{3A4F6131-954A-4F6B-BC51-8E9A8FDF27E9}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{3A4F6131-954A-4F6B-BC51-8E9A8FDF27E9}" name="Tabelle4" displayName="Tabelle4" ref="H1:L2" totalsRowShown="0">
+  <autoFilter ref="H1:L2" xr:uid="{3A4F6131-954A-4F6B-BC51-8E9A8FDF27E9}"/>
   <tableColumns count="5">
     <tableColumn id="5" xr3:uid="{24A2282B-9BBC-42A7-A34E-0FD0F404A30A}" name="Titel" dataDxfId="8"/>
     <tableColumn id="1" xr3:uid="{535AB875-9018-45C5-9F43-A4487869B22E}" name="InfoTextOben"/>
@@ -483,8 +510,8 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{29B5C5B2-6743-42FC-8083-8915EF4B9139}" name="Tabelle5" displayName="Tabelle5" ref="M1:N2" totalsRowShown="0">
-  <autoFilter ref="M1:N2" xr:uid="{29B5C5B2-6743-42FC-8083-8915EF4B9139}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{29B5C5B2-6743-42FC-8083-8915EF4B9139}" name="Tabelle5" displayName="Tabelle5" ref="N1:O2" totalsRowShown="0">
+  <autoFilter ref="N1:O2" xr:uid="{29B5C5B2-6743-42FC-8083-8915EF4B9139}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{BC4D296C-6336-436B-B850-FD3B6BC395F2}" name="FontFamily"/>
     <tableColumn id="2" xr3:uid="{5BA600E0-17A6-4994-B4BF-339A9FE90433}" name="FontSize"/>
@@ -811,26 +838,29 @@
   <sheetPr>
     <tabColor theme="1" tint="0.14999847407452621"/>
   </sheetPr>
-  <dimension ref="A1:N9"/>
+  <dimension ref="A1:O9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K21" sqref="K21"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.125" customWidth="1"/>
-    <col min="3" max="3" width="14" customWidth="1"/>
+    <col min="3" max="3" width="19" customWidth="1"/>
     <col min="4" max="4" width="17.25" customWidth="1"/>
-    <col min="5" max="6" width="20.25" customWidth="1"/>
-    <col min="7" max="8" width="33.125" customWidth="1"/>
-    <col min="10" max="10" width="33.125" customWidth="1"/>
-    <col min="11" max="11" width="102.875" customWidth="1"/>
+    <col min="5" max="5" width="18.875" customWidth="1"/>
+    <col min="6" max="6" width="20.25" customWidth="1"/>
+    <col min="7" max="7" width="17.25" customWidth="1"/>
+    <col min="8" max="8" width="20.25" customWidth="1"/>
+    <col min="9" max="10" width="33.125" customWidth="1"/>
     <col min="12" max="12" width="33.125" customWidth="1"/>
-    <col min="13" max="13" width="24.875" customWidth="1"/>
+    <col min="13" max="13" width="102.875" customWidth="1"/>
+    <col min="14" max="14" width="33.125" customWidth="1"/>
+    <col min="15" max="15" width="24.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -841,123 +871,139 @@
         <v>16</v>
       </c>
       <c r="E1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F1" t="s">
+        <v>70</v>
+      </c>
+      <c r="H1" t="s">
+        <v>65</v>
+      </c>
+      <c r="I1" t="s">
+        <v>56</v>
+      </c>
+      <c r="J1" t="s">
+        <v>57</v>
+      </c>
+      <c r="K1" t="s">
+        <v>58</v>
+      </c>
+      <c r="L1" t="s">
+        <v>59</v>
+      </c>
+      <c r="N1" t="s">
+        <v>67</v>
+      </c>
+      <c r="O1" t="s">
         <v>66</v>
       </c>
-      <c r="G1" t="s">
-        <v>77</v>
-      </c>
-      <c r="H1" t="s">
-        <v>68</v>
-      </c>
-      <c r="I1" t="s">
-        <v>69</v>
-      </c>
-      <c r="J1" t="s">
-        <v>70</v>
-      </c>
-      <c r="K1" t="s">
-        <v>71</v>
-      </c>
-      <c r="M1" t="s">
-        <v>79</v>
-      </c>
-      <c r="N1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" ht="18.2" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:15" ht="18.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>17</v>
+        <v>72</v>
       </c>
       <c r="D2" t="s">
-        <v>27</v>
-      </c>
-      <c r="E2" t="s">
-        <v>26</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="H2" t="s">
-        <v>72</v>
+        <v>74</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="F2" t="s">
+        <v>71</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>64</v>
       </c>
       <c r="I2" t="s">
-        <v>73</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="K2" t="s">
-        <v>75</v>
-      </c>
-      <c r="M2" t="s">
-        <v>80</v>
+        <v>60</v>
+      </c>
+      <c r="J2" t="s">
+        <v>61</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="L2" t="s">
+        <v>63</v>
       </c>
       <c r="N2" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" ht="18.2" customHeight="1" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+      <c r="O2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" ht="15.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>18</v>
+        <v>84</v>
       </c>
       <c r="D3" t="s">
-        <v>20</v>
-      </c>
-      <c r="E3" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+        <v>83</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="F3" t="s">
+        <v>75</v>
+      </c>
+      <c r="G3" s="3"/>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>10</v>
       </c>
       <c r="C4" t="s">
-        <v>19</v>
+        <v>77</v>
       </c>
       <c r="D4" t="s">
-        <v>28</v>
-      </c>
-      <c r="E4" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="F4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>25</v>
+        <v>81</v>
       </c>
       <c r="D5" t="s">
-        <v>29</v>
+        <v>80</v>
       </c>
       <c r="E5" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+        <v>79</v>
+      </c>
+      <c r="F5" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -965,11 +1011,12 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
   <tableParts count="4">
-    <tablePart r:id="rId1"/>
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
     <tablePart r:id="rId4"/>
+    <tablePart r:id="rId5"/>
   </tableParts>
 </worksheet>
 </file>
@@ -978,8 +1025,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F05469D6-429B-4FE2-AB98-8A05D5510F8C}">
   <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -1002,19 +1049,19 @@
         <v>3</v>
       </c>
       <c r="C1" t="s">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
       </c>
       <c r="E1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="F1" t="s">
         <v>0</v>
       </c>
       <c r="G1" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -1022,19 +1069,19 @@
         <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>17</v>
+        <v>72</v>
       </c>
       <c r="C2" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="D2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="F2">
         <v>6</v>
       </c>
       <c r="G2" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -1042,7 +1089,7 @@
         <v>8</v>
       </c>
       <c r="B3" t="s">
-        <v>17</v>
+        <v>72</v>
       </c>
       <c r="C3" t="s">
         <v>5</v>
@@ -1054,7 +1101,7 @@
         <v>6</v>
       </c>
       <c r="G3" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -1062,19 +1109,19 @@
         <v>8</v>
       </c>
       <c r="B4" t="s">
-        <v>18</v>
+        <v>84</v>
       </c>
       <c r="C4" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="D4" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="F4">
         <v>6</v>
       </c>
       <c r="G4" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -1082,19 +1129,19 @@
         <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>18</v>
+        <v>84</v>
       </c>
       <c r="C5" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="D5" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="F5">
         <v>6</v>
       </c>
       <c r="G5" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -1102,19 +1149,19 @@
         <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>19</v>
+        <v>77</v>
       </c>
       <c r="C6" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="D6" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="F6">
         <v>3</v>
       </c>
       <c r="G6" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -1122,19 +1169,19 @@
         <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>25</v>
+        <v>81</v>
       </c>
       <c r="C7" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
       <c r="D7" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="F7">
         <v>3</v>
       </c>
       <c r="G7" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -1142,19 +1189,19 @@
         <v>9</v>
       </c>
       <c r="B8" t="s">
-        <v>17</v>
+        <v>72</v>
       </c>
       <c r="C8" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="D8" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="F8">
         <v>6</v>
       </c>
       <c r="G8" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -1162,19 +1209,19 @@
         <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>17</v>
+        <v>72</v>
       </c>
       <c r="C9" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
       <c r="D9" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="F9">
         <v>6</v>
       </c>
       <c r="G9" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -1182,19 +1229,19 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>18</v>
+        <v>84</v>
       </c>
       <c r="C10" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="D10" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
       <c r="F10">
         <v>6</v>
       </c>
       <c r="G10" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -1202,19 +1249,19 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>19</v>
+        <v>77</v>
       </c>
       <c r="C11" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="D11" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="F11">
         <v>3</v>
       </c>
       <c r="G11" t="s">
-        <v>63</v>
+        <v>52</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -1222,19 +1269,19 @@
         <v>9</v>
       </c>
       <c r="B12" t="s">
-        <v>19</v>
+        <v>77</v>
       </c>
       <c r="C12" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="D12" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="F12">
         <v>6</v>
       </c>
       <c r="G12" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -1242,19 +1289,19 @@
         <v>9</v>
       </c>
       <c r="B13" t="s">
-        <v>25</v>
+        <v>81</v>
       </c>
       <c r="C13" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="D13" t="s">
-        <v>50</v>
+        <v>39</v>
       </c>
       <c r="F13">
         <v>3</v>
       </c>
       <c r="G13" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -1324,7 +1371,7 @@
         <v>6</v>
       </c>
       <c r="D1" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added info/warning texts and empty module option
</commit_message>
<xml_diff>
--- a/public/Modultafel_Template.xlsx
+++ b/public/Modultafel_Template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Laurent\IdeaProjects\Modultafel\public\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andri\IdeaProjects\Modultafel\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F901CE70-3219-45C7-BF90-7BAC60272341}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC429CF0-E184-43FA-8BED-EFBF268BD936}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20676" yWindow="0" windowWidth="17579" windowHeight="18842" activeTab="1" xr2:uid="{C0A2E809-DD1F-47D3-9648-758D3A48BE07}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" activeTab="1" xr2:uid="{C0A2E809-DD1F-47D3-9648-758D3A48BE07}"/>
   </bookViews>
   <sheets>
     <sheet name="Einstellungen" sheetId="2" r:id="rId1"/>
@@ -25,7 +25,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
@@ -34,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="82">
   <si>
     <t>ECTS</t>
   </si>
@@ -111,12 +113,6 @@
     <t>w.BA.XX.2SWEng.XX</t>
   </si>
   <si>
-    <t>Mathematik 1</t>
-  </si>
-  <si>
-    <t>w.BA.XX.2Mathe1-WIN.XX</t>
-  </si>
-  <si>
     <t>Business English 1</t>
   </si>
   <si>
@@ -175,9 +171,6 @@
   </si>
   <si>
     <t>https://modulmanagement.sml.zhaw.ch/StaticModDescAblage/Modulbeschreibung_w.BA.XX.2SWEng.XX.pdf</t>
-  </si>
-  <si>
-    <t>https://modulmanagement.sml.zhaw.ch/StaticModDescAblage/Modulbeschreibung_w.BA.XX.2Mathe1-WIN.XX.pdf</t>
   </si>
   <si>
     <t>https://modulmanagement.sml.zhaw.ch/StaticModDescAblage/Modulbeschreibung_w.BA.XX.2BusE1.XX.pdf</t>
@@ -297,7 +290,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -316,6 +309,14 @@
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -344,19 +345,23 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="9">
     <dxf>
@@ -521,8 +526,11 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{CF4ACF50-5041-4410-9F27-503054A8E586}" name="Tabelle1" displayName="Tabelle1" ref="A1:G1048575" totalsRowShown="0" dataDxfId="7">
-  <autoFilter ref="A1:G1048575" xr:uid="{CF4ACF50-5041-4410-9F27-503054A8E586}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{CF4ACF50-5041-4410-9F27-503054A8E586}" name="Tabelle1" displayName="Tabelle1" ref="A1:G1048576" totalsRowShown="0" dataDxfId="7">
+  <autoFilter ref="A1:G1048576" xr:uid="{CF4ACF50-5041-4410-9F27-503054A8E586}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G14">
+    <sortCondition ref="A1:A1048576"/>
+  </sortState>
   <tableColumns count="7">
     <tableColumn id="6" xr3:uid="{E6C1C015-3DB3-47F6-929A-743509FD5797}" name="Semester" dataDxfId="6"/>
     <tableColumn id="5" xr3:uid="{5E3B9891-0394-4C86-AC02-0F20186B6BAF}" name="Modulgruppe" dataDxfId="5"/>
@@ -539,7 +547,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -841,26 +849,27 @@
   <dimension ref="A1:O9"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="18.125" customWidth="1"/>
+    <col min="1" max="1" width="18.08984375" customWidth="1"/>
     <col min="3" max="3" width="19" customWidth="1"/>
-    <col min="4" max="4" width="17.25" customWidth="1"/>
-    <col min="5" max="5" width="18.875" customWidth="1"/>
-    <col min="6" max="6" width="20.25" customWidth="1"/>
-    <col min="7" max="7" width="17.25" customWidth="1"/>
-    <col min="8" max="8" width="20.25" customWidth="1"/>
-    <col min="9" max="10" width="33.125" customWidth="1"/>
-    <col min="12" max="12" width="33.125" customWidth="1"/>
-    <col min="13" max="13" width="102.875" customWidth="1"/>
-    <col min="14" max="14" width="33.125" customWidth="1"/>
-    <col min="15" max="15" width="24.875" customWidth="1"/>
+    <col min="4" max="4" width="17.26953125" customWidth="1"/>
+    <col min="5" max="5" width="18.90625" customWidth="1"/>
+    <col min="6" max="6" width="20.26953125" customWidth="1"/>
+    <col min="7" max="7" width="17.26953125" customWidth="1"/>
+    <col min="8" max="8" width="19.08984375" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="33.08984375" customWidth="1"/>
+    <col min="11" max="11" width="15.36328125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="33.08984375" customWidth="1"/>
+    <col min="13" max="13" width="102.90625" customWidth="1"/>
+    <col min="14" max="14" width="33.08984375" customWidth="1"/>
+    <col min="15" max="15" width="24.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -871,139 +880,139 @@
         <v>16</v>
       </c>
       <c r="E1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F1" t="s">
+        <v>67</v>
+      </c>
+      <c r="H1" t="s">
+        <v>62</v>
+      </c>
+      <c r="I1" t="s">
+        <v>53</v>
+      </c>
+      <c r="J1" t="s">
+        <v>54</v>
+      </c>
+      <c r="K1" t="s">
         <v>55</v>
       </c>
-      <c r="F1" t="s">
-        <v>70</v>
-      </c>
-      <c r="H1" t="s">
-        <v>65</v>
-      </c>
-      <c r="I1" t="s">
+      <c r="L1" t="s">
         <v>56</v>
       </c>
-      <c r="J1" t="s">
-        <v>57</v>
-      </c>
-      <c r="K1" t="s">
-        <v>58</v>
-      </c>
-      <c r="L1" t="s">
-        <v>59</v>
-      </c>
       <c r="N1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="O1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" ht="18.2" customHeight="1" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" ht="18.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="D2" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="F2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="I2" t="s">
+        <v>57</v>
+      </c>
+      <c r="J2" t="s">
+        <v>58</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="L2" t="s">
         <v>60</v>
       </c>
-      <c r="J2" t="s">
-        <v>61</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="L2" t="s">
-        <v>63</v>
-      </c>
       <c r="N2" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="O2" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" ht="15.65" customHeight="1" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="D3" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="F3" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="G3" s="3"/>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>10</v>
       </c>
       <c r="C4" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D4" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="F4" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D5" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="E5" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="F5" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -1023,25 +1032,25 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F05469D6-429B-4FE2-AB98-8A05D5510F8C}">
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12.625" customWidth="1"/>
+    <col min="1" max="1" width="12.6328125" customWidth="1"/>
     <col min="2" max="2" width="14" customWidth="1"/>
-    <col min="3" max="3" width="22.875" customWidth="1"/>
-    <col min="4" max="4" width="46.75" customWidth="1"/>
-    <col min="5" max="5" width="18.25" customWidth="1"/>
-    <col min="6" max="6" width="9.25" customWidth="1"/>
-    <col min="7" max="7" width="97.25" customWidth="1"/>
-    <col min="9" max="9" width="93.75" customWidth="1"/>
+    <col min="3" max="3" width="22.90625" customWidth="1"/>
+    <col min="4" max="4" width="46.7265625" customWidth="1"/>
+    <col min="5" max="5" width="18.26953125" customWidth="1"/>
+    <col min="6" max="6" width="9.26953125" customWidth="1"/>
+    <col min="7" max="7" width="97.26953125" customWidth="1"/>
+    <col min="9" max="9" width="93.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -1049,7 +1058,7 @@
         <v>3</v>
       </c>
       <c r="C1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
@@ -1061,75 +1070,63 @@
         <v>0</v>
       </c>
       <c r="G1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="C2" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="D2" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="F2">
         <v>6</v>
       </c>
       <c r="G2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>8</v>
       </c>
       <c r="B3" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C3" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="D3" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="F3">
         <v>6</v>
       </c>
       <c r="G3" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>8</v>
       </c>
       <c r="B4" t="s">
-        <v>84</v>
-      </c>
-      <c r="C4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D4" t="s">
-        <v>21</v>
-      </c>
-      <c r="F4">
-        <v>6</v>
-      </c>
-      <c r="G4" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C5" t="s">
         <v>24</v>
@@ -1141,167 +1138,179 @@
         <v>6</v>
       </c>
       <c r="G5" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="C6" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="D6" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="F6">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="G6" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>81</v>
+        <v>69</v>
       </c>
       <c r="C7" t="s">
-        <v>28</v>
+        <v>5</v>
       </c>
       <c r="D7" t="s">
-        <v>27</v>
+        <v>7</v>
       </c>
       <c r="F7">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="G7" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>9</v>
       </c>
       <c r="B8" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="C8" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="D8" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
       <c r="F8">
         <v>6</v>
       </c>
       <c r="G8" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C9" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D9" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="F9">
         <v>6</v>
       </c>
       <c r="G9" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>84</v>
+        <v>69</v>
       </c>
       <c r="C10" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="D10" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="F10">
         <v>6</v>
       </c>
       <c r="G10" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C11" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D11" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F11">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="G11" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>9</v>
       </c>
       <c r="B12" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="C12" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="D12" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="F12">
         <v>6</v>
       </c>
       <c r="G12" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>9</v>
       </c>
       <c r="B13" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="C13" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D13" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="F13">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="G13" t="s">
-        <v>54</v>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A14" s="4"/>
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="5" t="e">
+        <f>IF(Tabelle1[[#This Row],[Modulkuerzel]] &lt;&gt; "",HYPERLINK(CONCATENATE("https://modulmanagement.sml.zhaw.ch/StaticModDescAblage/Modulbeschreibung_",Tabelle1[[#This Row],[Modulkuerzel]],".pdf")), null)</f>
+        <v>#NAME?</v>
       </c>
     </row>
   </sheetData>
@@ -1313,30 +1322,24 @@
   </tableParts>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="4">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{C71FD47B-FA29-4E15-A390-7F74131AFF28}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{67DD0CEC-1861-49AF-8293-653FE548A64C}">
           <x14:formula1>
-            <xm:f>Einstellungen!$C$2:$C$358</xm:f>
+            <xm:f>Einstellungen!$A$2:$A$1048576</xm:f>
           </x14:formula1>
-          <xm:sqref>B1048576</xm:sqref>
+          <xm:sqref>A3:A4</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{C4B294B7-CD7F-497F-A32C-8C0979503DB7}">
           <x14:formula1>
             <xm:f>Einstellungen!$A:$A</xm:f>
           </x14:formula1>
-          <xm:sqref>B1048576 A2:A1048576</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{67DD0CEC-1861-49AF-8293-653FE548A64C}">
-          <x14:formula1>
-            <xm:f>Einstellungen!$A$2:$A$1048576</xm:f>
-          </x14:formula1>
-          <xm:sqref>A3</xm:sqref>
+          <xm:sqref>A2:A1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{E1B7B893-72C9-41C1-9921-547E295930C2}">
           <x14:formula1>
             <xm:f>Einstellungen!$C$2:$C$5</xm:f>
           </x14:formula1>
-          <xm:sqref>B2:B1048575</xm:sqref>
+          <xm:sqref>B2:B1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1352,15 +1355,15 @@
       <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="19" customWidth="1"/>
-    <col min="2" max="2" width="19.5" customWidth="1"/>
-    <col min="3" max="3" width="28.25" customWidth="1"/>
-    <col min="4" max="4" width="28.375" customWidth="1"/>
+    <col min="2" max="2" width="19.453125" customWidth="1"/>
+    <col min="3" max="3" width="28.26953125" customWidth="1"/>
+    <col min="4" max="4" width="28.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>1</v>
       </c>

</xml_diff>